<commit_message>
Configuracion data entry desde exel, manejo de hasmap
</commit_message>
<xml_diff>
--- a/src/test/resources/DataEntry/DataEntryTestCases.xlsx
+++ b/src/test/resources/DataEntry/DataEntryTestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PROJECTS FREELANCE\TESTING AUTOMATION\Selenium_Maven_TestNG\src\test\resources\DataEntry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35FD4880-BF14-41A9-A9D3-0CC5F044B523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36BB943-C0F4-433A-B006-ED67397FEDB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="3015" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4545" yWindow="3660" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataTestCases" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Ruby</t>
   </si>
@@ -61,6 +61,30 @@
   </si>
   <si>
     <t>TEST3</t>
+  </si>
+  <si>
+    <t>hola</t>
+  </si>
+  <si>
+    <t>mundo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tomas </t>
+  </si>
+  <si>
+    <t>vino}</t>
+  </si>
+  <si>
+    <t>TEST4</t>
+  </si>
+  <si>
+    <t>TEST5</t>
+  </si>
+  <si>
+    <t>Resultado</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -394,15 +418,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -412,19 +436,25 @@
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
+      <c r="D2" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -434,8 +464,11 @@
       <c r="C3" t="s">
         <v>7</v>
       </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -444,6 +477,37 @@
       </c>
       <c r="C4" t="s">
         <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>